<commit_message>
Design of analysis tables
</commit_message>
<xml_diff>
--- a/source/experiments/result_analysis.xlsx
+++ b/source/experiments/result_analysis.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\TDG Matemáticas\secure-svm\source\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61A9BE3-50C7-4A49-9836-48F23EA66700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696EE1DD-1CBC-48D3-BD2A-24133F291060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59365EC7-1685-4DC8-86FF-705BE4135883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{59365EC7-1685-4DC8-86FF-705BE4135883}"/>
   </bookViews>
   <sheets>
     <sheet name="Model selection" sheetId="1" r:id="rId1"/>
+    <sheet name="Column Experiments" sheetId="2" r:id="rId2"/>
+    <sheet name="Row Experiments" sheetId="3" r:id="rId3"/>
+    <sheet name="Difficulty Experiments" sheetId="4" r:id="rId4"/>
+    <sheet name="Real Experiments" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -53,13 +57,67 @@
   <si>
     <t>Least Squares</t>
   </si>
+  <si>
+    <t>Experiment name</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Training time - Secure (sec)</t>
+  </si>
+  <si>
+    <t>Training time - Clear (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Accuracy - Clear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train Accuracy - Clear </t>
+  </si>
+  <si>
+    <t>Test Accuracy - Secure (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train Accuracy - Secure (sec)  </t>
+  </si>
+  <si>
+    <t>Class separation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train Accuracy - Secure </t>
+  </si>
+  <si>
+    <t>Test Accuracy - Secure</t>
+  </si>
+  <si>
+    <t>Train percentage</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Secure</t>
+  </si>
+  <si>
+    <t>Training time</t>
+  </si>
+  <si>
+    <t>Data sent</t>
+  </si>
+  <si>
+    <t>Global data sent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -113,13 +171,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2765,16 +2827,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>899160</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2801,16 +2863,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2837,16 +2899,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3173,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18DF82E-5A11-4D71-8644-BB844A341599}">
   <dimension ref="B1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3274,4 +3336,419 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EBF4646-B330-4EB2-ADAE-391DC1ECED08}">
+  <dimension ref="C1:M4"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:M1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BAADC1-DB68-49C1-9BD8-9D64DC3FC6C6}">
+  <dimension ref="C1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F16:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437DAEAD-FBFF-41D6-9A07-C729BCDC9FFE}">
+  <dimension ref="C1:N4"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4544C202-F760-48C5-808B-1E418BC4CF42}">
+  <dimension ref="C3:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="7"/>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>